<commit_message>
positionnement énonce dans une 3e pages
</commit_message>
<xml_diff>
--- a/Data/Climat.xlsx
+++ b/Data/Climat.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23280" windowHeight="13200" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SI " sheetId="2" r:id="rId1"/>
     <sheet name="SI -erreur" sheetId="3" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="66">
   <si>
     <t>janvier</t>
   </si>
@@ -212,6 +213,12 @@
   </si>
   <si>
     <t>implémenter ces lois dans votre application précédente</t>
+  </si>
+  <si>
+    <t>SI sheet</t>
+  </si>
+  <si>
+    <t>SI- erreur sheet</t>
   </si>
 </sst>
 </file>
@@ -425,6 +432,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -750,20 +762,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O52"/>
+  <dimension ref="B1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:O58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -801,7 +813,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>12</v>
       </c>
@@ -842,7 +854,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -883,7 +895,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -924,7 +936,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>15</v>
       </c>
@@ -965,7 +977,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>16</v>
       </c>
@@ -1006,7 +1018,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>17</v>
       </c>
@@ -1047,7 +1059,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>18</v>
       </c>
@@ -1088,7 +1100,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>19</v>
       </c>
@@ -1129,7 +1141,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>20</v>
       </c>
@@ -1170,7 +1182,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>21</v>
       </c>
@@ -1211,7 +1223,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -1252,7 +1264,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>23</v>
       </c>
@@ -1294,7 +1306,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="17" spans="3:15">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>24</v>
       </c>
@@ -1335,7 +1347,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="18" spans="3:15">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>25</v>
       </c>
@@ -1376,7 +1388,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="19" spans="3:15">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>26</v>
       </c>
@@ -1417,7 +1429,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="20" spans="3:15">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>27</v>
       </c>
@@ -1458,7 +1470,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="21" spans="3:15">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>28</v>
       </c>
@@ -1499,7 +1511,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="22" spans="3:15">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>29</v>
       </c>
@@ -1540,7 +1552,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="23" spans="3:15">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>30</v>
       </c>
@@ -1581,7 +1593,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="24" spans="3:15">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>31</v>
       </c>
@@ -1623,7 +1635,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="25" spans="3:15">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>32</v>
       </c>
@@ -1664,7 +1676,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="26" spans="3:15">
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>33</v>
       </c>
@@ -1705,7 +1717,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="27" spans="3:15">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>34</v>
       </c>
@@ -1746,7 +1758,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="28" spans="3:15">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>35</v>
       </c>
@@ -1787,7 +1799,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="29" spans="3:15">
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>36</v>
       </c>
@@ -1828,7 +1840,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="30" spans="3:15">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>37</v>
       </c>
@@ -1869,7 +1881,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="31" spans="3:15">
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>38</v>
       </c>
@@ -1910,7 +1922,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="32" spans="3:15">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>39</v>
       </c>
@@ -1951,7 +1963,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>40</v>
       </c>
@@ -1990,7 +2002,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>41</v>
       </c>
@@ -2029,7 +2041,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>42</v>
       </c>
@@ -2058,65 +2070,6 @@
       <c r="N35" s="1"/>
       <c r="O35">
         <v>-5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15">
-      <c r="A42" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15">
-      <c r="B43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="B44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="B45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15">
-      <c r="B46" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15">
-      <c r="B47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15">
-      <c r="B48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2132,20 +2085,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O57"/>
+  <dimension ref="B1:O35"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:Q60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>12</v>
       </c>
@@ -2224,7 +2177,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -2265,7 +2218,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -2306,7 +2259,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>15</v>
       </c>
@@ -2347,7 +2300,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>16</v>
       </c>
@@ -2388,7 +2341,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>17</v>
       </c>
@@ -2429,7 +2382,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>18</v>
       </c>
@@ -2470,7 +2423,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>19</v>
       </c>
@@ -2511,7 +2464,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>20</v>
       </c>
@@ -2552,7 +2505,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>21</v>
       </c>
@@ -2593,7 +2546,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -2634,7 +2587,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>23</v>
       </c>
@@ -2676,7 +2629,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="17" spans="3:15">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>24</v>
       </c>
@@ -2717,7 +2670,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="18" spans="3:15">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>25</v>
       </c>
@@ -2758,7 +2711,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="19" spans="3:15">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>26</v>
       </c>
@@ -2799,7 +2752,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="20" spans="3:15">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>27</v>
       </c>
@@ -2840,7 +2793,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="21" spans="3:15">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>28</v>
       </c>
@@ -2881,7 +2834,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="22" spans="3:15">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>29</v>
       </c>
@@ -2922,7 +2875,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="23" spans="3:15">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>30</v>
       </c>
@@ -2963,7 +2916,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="24" spans="3:15">
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>31</v>
       </c>
@@ -3005,7 +2958,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="25" spans="3:15">
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>32</v>
       </c>
@@ -3046,7 +2999,7 @@
         <v>-33</v>
       </c>
     </row>
-    <row r="26" spans="3:15">
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>33</v>
       </c>
@@ -3087,7 +3040,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="27" spans="3:15">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>34</v>
       </c>
@@ -3128,7 +3081,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="28" spans="3:15">
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>35</v>
       </c>
@@ -3169,7 +3122,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="29" spans="3:15">
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>36</v>
       </c>
@@ -3210,7 +3163,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="30" spans="3:15">
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>37</v>
       </c>
@@ -3251,7 +3204,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="31" spans="3:15">
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>38</v>
       </c>
@@ -3292,7 +3245,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="32" spans="3:15">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>39</v>
       </c>
@@ -3333,7 +3286,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>40</v>
       </c>
@@ -3372,7 +3325,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>41</v>
       </c>
@@ -3411,7 +3364,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>42</v>
       </c>
@@ -3440,78 +3393,6 @@
       <c r="N35" s="1"/>
       <c r="O35">
         <v>-5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15">
-      <c r="A42" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15">
-      <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="B44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="B45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15">
-      <c r="B46" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15">
-      <c r="B47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15">
-      <c r="B48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2">
-      <c r="B54" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2">
-      <c r="B55" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2">
-      <c r="B56" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2">
-      <c r="B57" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3523,4 +3404,160 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>